<commit_message>
puxando do arquivo sumulas.xlsx
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Protocolo</t>
   </si>
@@ -64,8 +64,7 @@
     <t>82128/2020</t>
   </si>
   <si>
-    <t>
-36 3ª feira | 15/Set/2020 - Edição nº 10768 Particulares SÚMULA DE REQUERIMENTO DE LICENÇA DE INSTALAÇÃO J. C. MARQUES &amp; CIA LTDA, torna público que irá requerer ao IAP, a Licença de Instalação para ampliação da capacidade de armazenamento (tancagem) de combustíveis, a ser implantada na Avenida Saul Elkind, nº 4145, município de Londrina/PR. </t>
+    <t>36 3ª feira | 15/Set/2020 - Edição nº 10768 Particulares SÚMULA DE REQUERIMENTO DE LICENÇA DE INSTALAÇÃO J. C. MARQUES &amp; CIA LTDA, torna público que irá requerer ao IAP, a Licença de Instalação para ampliação da capacidade de armazenamento (tancagem) de combustíveis, a ser implantada na Avenida Saul Elkind, nº 4145, município de Londrina/PR. </t>
   </si>
   <si>
     <t>O J. C. MARQUES &amp; CIA LTDA,</t>
@@ -147,10 +146,6 @@
   </si>
   <si>
     <t>GMIL TRANSPORTES LTDA, </t>
-  </si>
-  <si>
-    <t>
-</t>
   </si>
 </sst>
 </file>
@@ -400,7 +395,7 @@
         <v>19</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>